<commit_message>
implements export data to excel
</commit_message>
<xml_diff>
--- a/src/main/java/excelFiles/APMacAddress.xlsx
+++ b/src/main/java/excelFiles/APMacAddress.xlsx
@@ -16,160 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Login.login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>password</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>username</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>country</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ubnt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>language</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>en_US</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>isFirstTimeLogin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>false</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>840</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tabName1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wirelessMode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ap</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chanelWidth</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SSID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>frequency</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2437</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AntennaGain</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>outputPower</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>newPassword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xalt12345</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tabName2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>updatedIPAddress</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.1.2.103</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>updatedNetmask</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>255.255.248.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.1.2.1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gatewayIP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tabName3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>U</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xmdt1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UBNT_configuration_M2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -189,7 +36,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,18 +45,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -217,39 +58,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -544,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1"/>
@@ -575,137 +391,7 @@
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="15.95" customHeight="1"/>
-    <row r="2" spans="1:21" s="5" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="3" customFormat="1" ht="15.95" customHeight="1">
-      <c r="A3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
+    <row r="1" s="2" customFormat="1" ht="15.95" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>